<commit_message>
optimize the game, setup UI
</commit_message>
<xml_diff>
--- a/Thiết lập tạo quái vật game Defender Monster Attack.xlsx
+++ b/Thiết lập tạo quái vật game Defender Monster Attack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Defense-Monster-Attack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD44DF-00A9-41C3-830B-FD6E7A82F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAE64BB-BF98-441B-8AA0-06EB85D9EC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,6 +1289,20 @@
       </c>
       <c r="K42" s="1"/>
     </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="E43">
+        <v>8</v>
+      </c>
+      <c r="H43">
+        <v>10</v>
+      </c>
+      <c r="K43">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="N1:O1"/>
@@ -1300,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FFBAB41-C580-49C5-91A9-ACD0F1FE51B1}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,19 +1365,27 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
       <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1">
+        <v>5</v>
+      </c>
       <c r="N2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1381,19 +1403,27 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
       <c r="J3" s="1">
         <v>1</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
       <c r="N3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1492,37 +1522,53 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
       <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
       <c r="G7" s="1">
         <v>5</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
       <c r="J7" s="1">
         <v>5</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
       <c r="D8" s="1">
         <v>6</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
       <c r="G8" s="1">
         <v>6</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
       <c r="J8" s="1">
         <v>6</v>
       </c>
-      <c r="K8" s="1"/>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -1582,37 +1628,53 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
       <c r="D12" s="1">
         <v>10</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
       <c r="G12" s="1">
         <v>10</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>4</v>
+      </c>
       <c r="J12" s="1">
         <v>10</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
       <c r="D13" s="1">
         <v>11</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
       <c r="G13" s="1">
         <v>11</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
       <c r="J13" s="1">
         <v>11</v>
       </c>
-      <c r="K13" s="1"/>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1672,37 +1734,53 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
       <c r="D17" s="1">
         <v>15</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
       <c r="G17" s="1">
         <v>15</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
       <c r="J17" s="1">
         <v>15</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
       <c r="D18" s="1">
         <v>16</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
       <c r="G18" s="1">
         <v>16</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
       <c r="J18" s="1">
         <v>16</v>
       </c>
-      <c r="K18" s="1"/>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1762,37 +1840,53 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
       <c r="D22" s="1">
         <v>20</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1">
+        <v>3</v>
+      </c>
       <c r="G22" s="1">
         <v>20</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1">
+        <v>3</v>
+      </c>
       <c r="J22" s="1">
         <v>20</v>
       </c>
-      <c r="K22" s="1"/>
+      <c r="K22" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
       <c r="D23" s="1">
         <v>21</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
       <c r="G23" s="1">
         <v>21</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
       <c r="J23" s="1">
         <v>21</v>
       </c>
-      <c r="K23" s="1"/>
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -1852,37 +1946,53 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
       <c r="D27" s="1">
         <v>25</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>2</v>
+      </c>
       <c r="G27" s="1">
         <v>25</v>
       </c>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1">
+        <v>2</v>
+      </c>
       <c r="J27" s="1">
         <v>25</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="K27" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
       <c r="D28" s="1">
         <v>26</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
       <c r="G28" s="1">
         <v>26</v>
       </c>
-      <c r="H28" s="1"/>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
       <c r="J28" s="1">
         <v>26</v>
       </c>
-      <c r="K28" s="1"/>
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -1942,37 +2052,53 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1">
+        <v>2</v>
+      </c>
       <c r="D32" s="1">
         <v>30</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>2</v>
+      </c>
       <c r="G32" s="1">
         <v>30</v>
       </c>
-      <c r="H32" s="1"/>
+      <c r="H32" s="1">
+        <v>2</v>
+      </c>
       <c r="J32" s="1">
         <v>30</v>
       </c>
-      <c r="K32" s="1"/>
+      <c r="K32" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
       <c r="D33" s="1">
         <v>31</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
       <c r="G33" s="1">
         <v>31</v>
       </c>
-      <c r="H33" s="1"/>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
       <c r="J33" s="1">
         <v>31</v>
       </c>
-      <c r="K33" s="1"/>
+      <c r="K33" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -2135,6 +2261,21 @@
         <v>40</v>
       </c>
       <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f>11+14+10+6+7</f>
+        <v>48</v>
+      </c>
+      <c r="E43">
+        <v>48</v>
+      </c>
+      <c r="H43">
+        <v>48</v>
+      </c>
+      <c r="K43">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2146,10 +2287,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682743E1-F3EA-4C1A-81CC-4A6135FA478B}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3020,6 +3161,20 @@
       </c>
       <c r="K42" s="1"/>
     </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>16</v>
+      </c>
+      <c r="H43">
+        <v>9</v>
+      </c>
+      <c r="K43">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="N1:O1"/>
@@ -3031,10 +3186,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271C742D-2859-41B8-8014-C0CB801935EF}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3909,6 +4064,20 @@
       </c>
       <c r="K42" s="1"/>
     </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>15</v>
+      </c>
+      <c r="H43">
+        <v>20</v>
+      </c>
+      <c r="K43">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="N1:O1"/>
@@ -3919,10 +4088,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BB8E53-FD37-4674-BC89-2D66D5E6BAAA}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4797,6 +4966,20 @@
       </c>
       <c r="K42" s="1"/>
     </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="H43">
+        <v>13</v>
+      </c>
+      <c r="K43">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="N1:O1"/>
@@ -4807,10 +4990,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86861F2-EFD2-4F9B-ADF9-92F04F5FD710}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5691,6 +5874,20 @@
       </c>
       <c r="K42" s="1"/>
     </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>16</v>
+      </c>
+      <c r="E43">
+        <v>16</v>
+      </c>
+      <c r="H43">
+        <v>10</v>
+      </c>
+      <c r="K43">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="N1:O1"/>
@@ -5701,10 +5898,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC46E38B-D71D-4184-B0C4-EBFD1E742E01}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6585,6 +6782,20 @@
       </c>
       <c r="K42" s="1"/>
     </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>30</v>
+      </c>
+      <c r="E43">
+        <v>22</v>
+      </c>
+      <c r="H43">
+        <v>16</v>
+      </c>
+      <c r="K43">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="N1:O1"/>
@@ -6595,10 +6806,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9B6F02-F87F-425E-A663-809452A70534}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6658,7 +6869,9 @@
       <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
       <c r="N2" s="2" t="s">
         <v>3</v>
       </c>
@@ -6714,7 +6927,9 @@
       <c r="G4" s="1">
         <v>2</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
       <c r="J4" s="1">
         <v>2</v>
       </c>
@@ -6787,11 +7002,15 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
       <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
       <c r="G7" s="1">
         <v>5</v>
       </c>
@@ -6799,7 +7018,9 @@
       <c r="J7" s="1">
         <v>5</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -6885,11 +7106,15 @@
       <c r="G12" s="1">
         <v>10</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
       <c r="J12" s="1">
         <v>10</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -6967,11 +7192,15 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
       <c r="D17" s="1">
         <v>15</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
       <c r="G17" s="1">
         <v>15</v>
       </c>
@@ -6979,7 +7208,9 @@
       <c r="J17" s="1">
         <v>15</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -7065,11 +7296,15 @@
       <c r="G22" s="1">
         <v>20</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1">
+        <v>2</v>
+      </c>
       <c r="J22" s="1">
         <v>20</v>
       </c>
-      <c r="K22" s="1"/>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -7151,7 +7386,9 @@
       <c r="D27" s="1">
         <v>25</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>3</v>
+      </c>
       <c r="G27" s="1">
         <v>25</v>
       </c>
@@ -7159,7 +7396,9 @@
       <c r="J27" s="1">
         <v>25</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -7209,7 +7448,9 @@
       <c r="G30" s="1">
         <v>28</v>
       </c>
-      <c r="H30" s="1"/>
+      <c r="H30" s="1">
+        <v>2</v>
+      </c>
       <c r="J30" s="1">
         <v>28</v>
       </c>
@@ -7249,7 +7490,9 @@
       <c r="J32" s="1">
         <v>30</v>
       </c>
-      <c r="K32" s="1"/>
+      <c r="K32" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -7430,6 +7673,20 @@
         <v>40</v>
       </c>
       <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>14</v>
+      </c>
+      <c r="E43">
+        <v>15</v>
+      </c>
+      <c r="H43">
+        <v>12</v>
+      </c>
+      <c r="K43">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7441,10 +7698,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446DADE8-E764-4D66-8A9D-060A4C36581B}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:R6"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7492,19 +7749,27 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
       <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1">
+        <v>5</v>
+      </c>
       <c r="N2" s="2" t="s">
         <v>3</v>
       </c>
@@ -7522,7 +7787,9 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
@@ -7556,7 +7823,9 @@
       <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
       <c r="G4" s="1">
         <v>2</v>
       </c>
@@ -7587,7 +7856,9 @@
       <c r="G5" s="1">
         <v>3</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
       <c r="J5" s="1">
         <v>3</v>
       </c>
@@ -7606,7 +7877,9 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
       <c r="D6" s="1">
         <v>4</v>
       </c>
@@ -7618,7 +7891,9 @@
       <c r="J6" s="1">
         <v>4</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
       <c r="N6" s="2" t="s">
         <v>7</v>
       </c>
@@ -7637,7 +7912,9 @@
       <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
       <c r="G7" s="1">
         <v>5</v>
       </c>
@@ -7659,7 +7936,9 @@
       <c r="G8" s="1">
         <v>6</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
       <c r="J8" s="1">
         <v>6</v>
       </c>
@@ -7681,7 +7960,9 @@
       <c r="J9" s="1">
         <v>7</v>
       </c>
-      <c r="K9" s="1"/>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -7723,25 +8004,35 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
       <c r="D12" s="1">
         <v>10</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
       <c r="G12" s="1">
         <v>10</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
       <c r="J12" s="1">
         <v>10</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
       <c r="D13" s="1">
         <v>11</v>
       </c>
@@ -7763,7 +8054,9 @@
       <c r="D14" s="1">
         <v>12</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
       <c r="G14" s="1">
         <v>12</v>
       </c>
@@ -7785,7 +8078,9 @@
       <c r="G15" s="1">
         <v>13</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
       <c r="J15" s="1">
         <v>13</v>
       </c>
@@ -7795,7 +8090,9 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
       <c r="D16" s="1">
         <v>14</v>
       </c>
@@ -7807,7 +8104,9 @@
       <c r="J16" s="1">
         <v>14</v>
       </c>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -7817,7 +8116,9 @@
       <c r="D17" s="1">
         <v>15</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
       <c r="G17" s="1">
         <v>15</v>
       </c>
@@ -7839,7 +8140,9 @@
       <c r="G18" s="1">
         <v>16</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
       <c r="J18" s="1">
         <v>16</v>
       </c>
@@ -7849,7 +8152,9 @@
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
       <c r="D19" s="1">
         <v>17</v>
       </c>
@@ -7861,7 +8166,9 @@
       <c r="J19" s="1">
         <v>17</v>
       </c>
-      <c r="K19" s="1"/>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -7871,7 +8178,9 @@
       <c r="D20" s="1">
         <v>18</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
       <c r="G20" s="1">
         <v>18</v>
       </c>
@@ -7893,7 +8202,9 @@
       <c r="G21" s="1">
         <v>19</v>
       </c>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
       <c r="J21" s="1">
         <v>19</v>
       </c>
@@ -7903,7 +8214,9 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
       <c r="D22" s="1">
         <v>20</v>
       </c>
@@ -7915,7 +8228,9 @@
       <c r="J22" s="1">
         <v>20</v>
       </c>
-      <c r="K22" s="1"/>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -7925,7 +8240,9 @@
       <c r="D23" s="1">
         <v>21</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
       <c r="G23" s="1">
         <v>21</v>
       </c>
@@ -7947,7 +8264,9 @@
       <c r="G24" s="1">
         <v>22</v>
       </c>
-      <c r="H24" s="1"/>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
       <c r="J24" s="1">
         <v>22</v>
       </c>
@@ -7957,7 +8276,9 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
       <c r="D25" s="1">
         <v>23</v>
       </c>
@@ -7969,7 +8290,9 @@
       <c r="J25" s="1">
         <v>23</v>
       </c>
-      <c r="K25" s="1"/>
+      <c r="K25" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -7979,7 +8302,9 @@
       <c r="D26" s="1">
         <v>24</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
       <c r="G26" s="1">
         <v>24</v>
       </c>
@@ -8001,7 +8326,9 @@
       <c r="G27" s="1">
         <v>25</v>
       </c>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
       <c r="J27" s="1">
         <v>25</v>
       </c>
@@ -8011,7 +8338,9 @@
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
       <c r="D28" s="1">
         <v>26</v>
       </c>
@@ -8023,7 +8352,9 @@
       <c r="J28" s="1">
         <v>26</v>
       </c>
-      <c r="K28" s="1"/>
+      <c r="K28" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -8033,7 +8364,9 @@
       <c r="D29" s="1">
         <v>27</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
       <c r="G29" s="1">
         <v>27</v>
       </c>
@@ -8055,7 +8388,9 @@
       <c r="G30" s="1">
         <v>28</v>
       </c>
-      <c r="H30" s="1"/>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
       <c r="J30" s="1">
         <v>28</v>
       </c>
@@ -8065,7 +8400,9 @@
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
       <c r="D31" s="1">
         <v>29</v>
       </c>
@@ -8077,7 +8414,9 @@
       <c r="J31" s="1">
         <v>29</v>
       </c>
-      <c r="K31" s="1"/>
+      <c r="K31" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -8087,7 +8426,9 @@
       <c r="D32" s="1">
         <v>30</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
       <c r="G32" s="1">
         <v>30</v>
       </c>
@@ -8109,7 +8450,9 @@
       <c r="G33" s="1">
         <v>31</v>
       </c>
-      <c r="H33" s="1"/>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
       <c r="J33" s="1">
         <v>31</v>
       </c>
@@ -8131,7 +8474,9 @@
       <c r="J34" s="1">
         <v>32</v>
       </c>
-      <c r="K34" s="1"/>
+      <c r="K34" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -8276,6 +8621,21 @@
         <v>40</v>
       </c>
       <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f>11*2+9</f>
+        <v>31</v>
+      </c>
+      <c r="E43">
+        <v>31</v>
+      </c>
+      <c r="H43">
+        <v>31</v>
+      </c>
+      <c r="K43">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8287,10 +8647,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE1B392-6942-4A86-82E4-A963F3E3CCB7}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:R6"/>
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8338,19 +8698,27 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1">
+        <v>3</v>
+      </c>
       <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1">
+        <v>2</v>
+      </c>
       <c r="N2" s="2" t="s">
         <v>3</v>
       </c>
@@ -8479,19 +8847,27 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
       <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
       <c r="G7" s="1">
         <v>5</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
       <c r="J7" s="1">
         <v>5</v>
       </c>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -8569,19 +8945,27 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
       <c r="D12" s="1">
         <v>10</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
       <c r="G12" s="1">
         <v>10</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
       <c r="J12" s="1">
         <v>10</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -8659,19 +9043,27 @@
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
       <c r="D17" s="1">
         <v>15</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
       <c r="G17" s="1">
         <v>15</v>
       </c>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
       <c r="J17" s="1">
         <v>15</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -8749,19 +9141,27 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
       <c r="D22" s="1">
         <v>20</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1">
+        <v>2</v>
+      </c>
       <c r="G22" s="1">
         <v>20</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
       <c r="J22" s="1">
         <v>20</v>
       </c>
-      <c r="K22" s="1"/>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -8839,19 +9239,27 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1">
+        <v>3</v>
+      </c>
       <c r="D27" s="1">
         <v>25</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>2</v>
+      </c>
       <c r="G27" s="1">
         <v>25</v>
       </c>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
       <c r="J27" s="1">
         <v>25</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -8929,11 +9337,15 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1">
+        <v>2</v>
+      </c>
       <c r="D32" s="1">
         <v>30</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
       <c r="G32" s="1">
         <v>30</v>
       </c>
@@ -9122,6 +9534,23 @@
         <v>40</v>
       </c>
       <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f>22+14+10+3</f>
+        <v>49</v>
+      </c>
+      <c r="E43">
+        <f>14+10+6+1</f>
+        <v>31</v>
+      </c>
+      <c r="H43">
+        <f>10+6+2</f>
+        <v>18</v>
+      </c>
+      <c r="K43">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>